<commit_message>
Adding all work till now
</commit_message>
<xml_diff>
--- a/Blue_star_data.xlsx
+++ b/Blue_star_data.xlsx
@@ -421,10 +421,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B1:W18"/>
+  <dimension ref="B1:W17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="83" workbookViewId="0">
-      <selection activeCell="W16" sqref="W16:W17"/>
+    <sheetView tabSelected="1" zoomScale="81" workbookViewId="0">
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
@@ -1815,10 +1815,8 @@
           <t>11111111</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>11111111</t>
-        </is>
+      <c r="D15" t="n">
+        <v>11111111</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
@@ -2100,73 +2098,6 @@
       <c r="W17">
         <f>79-V17</f>
         <v/>
-      </c>
-    </row>
-    <row r="18">
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>11010101</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>01001110</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>11010111</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>00101111</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>11111010</t>
-        </is>
-      </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>10011000</t>
-        </is>
-      </c>
-      <c r="H18" t="inlineStr">
-        <is>
-          <t>11111111</t>
-        </is>
-      </c>
-      <c r="I18" t="inlineStr">
-        <is>
-          <t>11111011</t>
-        </is>
-      </c>
-      <c r="J18" t="inlineStr">
-        <is>
-          <t>11111111</t>
-        </is>
-      </c>
-      <c r="K18" t="inlineStr">
-        <is>
-          <t>01111111</t>
-        </is>
-      </c>
-      <c r="L18" t="inlineStr">
-        <is>
-          <t>01100110</t>
-        </is>
-      </c>
-      <c r="M18" t="inlineStr">
-        <is>
-          <t>11111101</t>
-        </is>
-      </c>
-      <c r="N18" t="inlineStr">
-        <is>
-          <t>11011100</t>
-        </is>
       </c>
     </row>
   </sheetData>
@@ -2180,14 +2111,15 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B2:Q4"/>
+  <dimension ref="B1:Q19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q2" sqref="Q2"/>
+    <sheetView topLeftCell="A2" zoomScale="71" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
   <sheetData>
+    <row r="1"/>
     <row r="2">
       <c r="B2" t="inlineStr">
         <is>
@@ -2196,17 +2128,17 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>11111110</t>
+          <t>11111111</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>11111111</t>
+          <t>11010111</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>11011011</t>
+          <t>00110011</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -2241,12 +2173,12 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>00010000</t>
+          <t>01000001</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>11111110</t>
+          <t>11111101</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
@@ -2256,7 +2188,7 @@
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>fan3</t>
         </is>
       </c>
     </row>
@@ -2273,12 +2205,12 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>11111111</t>
+          <t>11010111</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>11011011</t>
+          <t>00110111</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -2313,17 +2245,22 @@
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>00010001</t>
+          <t>01000101</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>11111110</t>
+          <t>11111101</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
         <is>
           <t>11011100</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>fan2</t>
         </is>
       </c>
     </row>
@@ -2340,55 +2277,1120 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
+          <t>11010111</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>00111011</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>11111010</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>01011111</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>11111010</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>01011111</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>11111111</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>01111111</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>01001001</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>11111101</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>11011100</t>
+        </is>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>fan1</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>11010101</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>11111111</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>11010111</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>00101111</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>11111010</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>01011111</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>11111010</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>01011111</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>11111111</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>01111111</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>00111101</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>11111101</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>11011100</t>
+        </is>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>auto</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>11010101</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>11111111</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>11010111</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>00111011</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>11111010</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>01011111</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>11111010</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>01011111</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>11111111</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>01111111</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>01001001</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>11111101</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>11011100</t>
+        </is>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>modecold</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>11010101</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>11111111</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>10110111</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>00111011</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>11111010</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>01011111</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>11111010</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>01011111</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>11111111</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>01111111</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>00101001</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>11111101</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>11011100</t>
+        </is>
+      </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>modecool</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>11010101</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>11111111</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>10010111</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>00111011</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>11111010</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>01011111</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>11111010</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>01011111</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>11111111</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>01111111</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>00001001</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>11111101</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>11011100</t>
+        </is>
+      </c>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>modefan</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>11010101</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>11111111</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>11110111</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>00111011</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>11111010</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>01011111</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>11111010</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>01011111</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>11111111</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>01111111</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>01101001</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>11111101</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>11011100</t>
+        </is>
+      </c>
+      <c r="Q9" t="inlineStr">
+        <is>
+          <t>modeheat</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>11010101</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>11111111</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>11010111</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>00101111</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>11111010</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>01011111</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>11111010</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>01011111</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>11111111</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>01111111</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>00111101</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>11111101</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>11011100</t>
+        </is>
+      </c>
+      <c r="Q10" t="inlineStr">
+        <is>
+          <t>swing1</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>11010101</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>11111111</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>11010111</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>11001111</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>11111010</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>01011111</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>11111010</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>01011111</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>11111111</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>01111111</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>11011101</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>11111101</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>11011100</t>
+        </is>
+      </c>
+      <c r="Q11" t="inlineStr">
+        <is>
+          <t>swing2</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>11010101</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>11111111</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>11010111</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>10101111</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>11111010</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>01011111</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>11111010</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>01011111</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>11111111</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>01111111</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>10111101</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>11111101</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>11011100</t>
+        </is>
+      </c>
+      <c r="Q12" t="inlineStr">
+        <is>
+          <t>swing3</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>11010101</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>11111111</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>11010111</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>10001111</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>11111010</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>01011111</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>11111010</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>01011111</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>11111111</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>01111111</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>10011101</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>11111101</t>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>11011100</t>
+        </is>
+      </c>
+      <c r="Q13" t="inlineStr">
+        <is>
+          <t>swing4</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>11010101</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>11111111</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>11010111</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>01101111</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>11111010</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>01011111</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>11111010</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>01011111</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>11111111</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>01111111</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>01111101</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>11111101</t>
+        </is>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>11011100</t>
+        </is>
+      </c>
+      <c r="Q14" t="inlineStr">
+        <is>
+          <t>swing5</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>11010101</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>11111111</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>11010111</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>01001111</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>11111010</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>01011111</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>11111010</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>01011111</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>11111111</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>01111111</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>01011101</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>11111101</t>
+        </is>
+      </c>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>11011100</t>
+        </is>
+      </c>
+      <c r="Q15" t="inlineStr">
+        <is>
+          <t>swing6</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>11010101</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
           <t>11111110</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>11011011</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>11111010</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>01011111</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>11111010</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>01011111</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>11111111</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>11010111</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>01001111</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>11111010</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>01011111</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>11111010</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>01011111</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>11111111</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
         <is>
           <t>01111111</t>
         </is>
       </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>00010000</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>01011100</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>11111101</t>
+        </is>
+      </c>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>11011100</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>11010101</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
         <is>
           <t>11111110</t>
         </is>
       </c>
-      <c r="N4" t="inlineStr">
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>11010111</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>01001111</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>11111010</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>01011111</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>11111010</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>01011111</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>11111111</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>01111111</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>01011100</t>
+        </is>
+      </c>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>11111101</t>
+        </is>
+      </c>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>11011100</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>11010101</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>11111110</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>11010111</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>01001111</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>11111010</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>01011111</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>11111010</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>01011111</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>11111111</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>01111111</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>01011100</t>
+        </is>
+      </c>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>11111101</t>
+        </is>
+      </c>
+      <c r="N18" t="inlineStr">
+        <is>
+          <t>11011100</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>11010101</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>11111110</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>11010111</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>01010111</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>11111010</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>01011111</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>11111010</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>01011111</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>11111111</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>01111111</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>01100100</t>
+        </is>
+      </c>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>11111101</t>
+        </is>
+      </c>
+      <c r="N19" t="inlineStr">
         <is>
           <t>11011100</t>
         </is>

</xml_diff>